<commit_message>
Changes to reproduce new paper figures
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_errorVary.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_errorVary.xlsx
@@ -463,10 +463,10 @@
         <v>0.33</v>
       </c>
       <c r="B2">
-        <v>0.429</v>
+        <v>0.363</v>
       </c>
       <c r="C2">
-        <v>0.231</v>
+        <v>0.297</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -481,37 +481,37 @@
         <v>2.31</v>
       </c>
       <c r="H2">
-        <v>3.003</v>
+        <v>2.541</v>
       </c>
       <c r="I2">
-        <v>1.617</v>
+        <v>2.079</v>
       </c>
       <c r="J2">
         <v>63</v>
       </c>
       <c r="K2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="L2">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="M2">
         <v>0.2045973560979079</v>
       </c>
       <c r="N2">
-        <v>0.300815382785397</v>
+        <v>0.2393131875437522</v>
       </c>
       <c r="O2">
-        <v>0.08437673228171276</v>
+        <v>0.166830908040689</v>
       </c>
       <c r="P2">
         <v>0.8641481196490648</v>
       </c>
       <c r="Q2">
-        <v>0.9406845604581326</v>
+        <v>0.8978683829373846</v>
       </c>
       <c r="R2">
-        <v>0.6483325800579999</v>
+        <v>0.8170792379544533</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -528,46 +528,46 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>9.1</v>
+        <v>7.700000000000001</v>
       </c>
       <c r="F3">
-        <v>4.899999999999999</v>
+        <v>6.3</v>
       </c>
       <c r="G3">
         <v>2.31</v>
       </c>
       <c r="H3">
-        <v>3.003</v>
+        <v>2.541</v>
       </c>
       <c r="I3">
-        <v>1.617</v>
+        <v>2.079</v>
       </c>
       <c r="J3">
         <v>63</v>
       </c>
       <c r="K3">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L3">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="M3">
         <v>0.2045973560979079</v>
       </c>
       <c r="N3">
-        <v>0.3007680032180108</v>
+        <v>0.2393692844097636</v>
       </c>
       <c r="O3">
-        <v>0.0843518650899165</v>
+        <v>0.1669656336268933</v>
       </c>
       <c r="P3">
         <v>0.8641481196490648</v>
       </c>
       <c r="Q3">
-        <v>0.9406842222588339</v>
+        <v>0.8978681217589644</v>
       </c>
       <c r="R3">
-        <v>0.6509816340808184</v>
+        <v>0.8170831300264577</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -575,55 +575,55 @@
         <v>0.33</v>
       </c>
       <c r="B4">
-        <v>0.429</v>
+        <v>0.363</v>
       </c>
       <c r="C4">
-        <v>0.231</v>
+        <v>0.297</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>9.1</v>
+        <v>7.700000000000001</v>
       </c>
       <c r="F4">
-        <v>4.899999999999999</v>
+        <v>6.3</v>
       </c>
       <c r="G4">
         <v>2.31</v>
       </c>
       <c r="H4">
-        <v>3.9039</v>
+        <v>2.795100000000001</v>
       </c>
       <c r="I4">
-        <v>1.1319</v>
+        <v>1.8711</v>
       </c>
       <c r="J4">
         <v>63</v>
       </c>
       <c r="K4">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="L4">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="M4">
         <v>0.2045973560979079</v>
       </c>
       <c r="N4">
-        <v>0.3948931506643786</v>
+        <v>0.2744746858349662</v>
       </c>
       <c r="O4">
-        <v>0.001832682008754684</v>
+        <v>0.1307057700218693</v>
       </c>
       <c r="P4">
         <v>0.8641481196490648</v>
       </c>
       <c r="Q4">
-        <v>0.9780315117652149</v>
+        <v>0.9245436742198752</v>
       </c>
       <c r="R4">
-        <v>0.01672357170321865</v>
+        <v>0.7577615324283289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>